<commit_message>
More fixes. Now seems to be stable.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/08_caso_energia_eu_new_commands_CASE_SENSITIVE.xlsx
+++ b/backend_tests/z_input_files/v2/08_caso_energia_eu_new_commands_CASE_SENSITIVE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="392">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -157,246 +157,258 @@
     <t xml:space="preserve">C19</t>
   </si>
   <si>
+    <t xml:space="preserve">c20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31_C32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E37-E39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O-Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nama_10_a64_e</t>
+  </si>
+  <si>
     <t xml:space="preserve">C20</t>
   </si>
   <si>
-    <t xml:space="preserve">C21</t>
-  </si>
-  <si>
     <t xml:space="preserve">C22</t>
   </si>
   <si>
-    <t xml:space="preserve">C23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C31_C32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E37-E39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O-Q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R-U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nama_10_a64_e</t>
-  </si>
-  <si>
     <t xml:space="preserve">InputDataset</t>
   </si>
   <si>
     <t xml:space="preserve">AvailableAtDateTime</t>
   </si>
   <si>
+    <t xml:space="preserve">freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA_ITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartPeriod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EndPeriod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultDimensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultMeasures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultMeasuresAggregation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultMeasureNames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLV05_MEUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chain linked volumes (2005), million euro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agriculture, forestry and fishing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value added, gross</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">af</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agriculture/Forestry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME_PERIOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBS_VALUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ds1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLV05_MNAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chain linked volumes (2005), million units of national currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crop and animal production, hunting and related service activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2A3N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operating surplus and mixed income, net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy &amp; Mining</t>
+  </si>
+  <si>
     <t xml:space="preserve">FREQ</t>
   </si>
   <si>
+    <t xml:space="preserve">CLV10_MEUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chain linked volumes (2010), million euro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forestry and logging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compensation of employees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food &amp; Tobacco</t>
+  </si>
+  <si>
     <t xml:space="preserve">UNIT</t>
   </si>
   <si>
-    <t xml:space="preserve">NA_ITEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartPeriod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndPeriod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResultDimensions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResultMeasures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResultMeasuresAggregation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResultMeasureNames</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResultName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLV05_MEUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chain linked volumes (2005), million euro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agriculture, forestry and fishing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value added, gross</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Albania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agriculture/Forestry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIME_PERIOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBS_VALUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ds1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLV05_MNAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chain linked volumes (2005), million units of national currency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crop and animal production, hunting and related service activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B2A3N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operating surplus and mixed income, net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Austria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy &amp; Mining</t>
-  </si>
-  <si>
-    <t xml:space="preserve">freq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLV10_MEUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chain linked volumes (2010), million euro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forestry and logging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compensation of employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bosnia and Herzegovina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food &amp; Tobacco</t>
-  </si>
-  <si>
     <t xml:space="preserve">CLV10_MNAC</t>
   </si>
   <si>
@@ -649,7 +661,7 @@
     <t xml:space="preserve">Land transport and transport via pipelines</t>
   </si>
   <si>
-    <t xml:space="preserve">uk</t>
+    <t xml:space="preserve">UK</t>
   </si>
   <si>
     <t xml:space="preserve">United Kingdom</t>
@@ -1181,9 +1193,6 @@
   </si>
   <si>
     <t xml:space="preserve">Wholesale and retail trade and repair of motor vehicles and motorcycles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UK</t>
   </si>
   <si>
     <t xml:space="preserve">Wholesale trade, except of motor vehicles and motorcycles</t>
@@ -1546,8 +1555,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1775,7 +1784,7 @@
       <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -2439,7 +2448,7 @@
         <v>35</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>12</v>
@@ -2473,7 +2482,7 @@
         <v>35</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>12</v>
@@ -3050,8 +3059,8 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3077,17 +3086,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6" t="s">
@@ -3095,11 +3104,11 @@
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L1" s="6"/>
       <c r="M1" s="5" t="s">
@@ -3107,26 +3116,26 @@
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3137,37 +3146,37 @@
         <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="O2" s="4" t="n">
         <v>2016</v>
@@ -3177,55 +3186,55 @@
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="U2" s="4"/>
       <c r="V2" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
@@ -3233,40 +3242,40 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
@@ -3274,34 +3283,34 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="4" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
@@ -3315,40 +3324,40 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
@@ -3356,40 +3365,40 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="4" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
@@ -3399,34 +3408,34 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -3442,30 +3451,30 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -3479,30 +3488,30 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -3516,30 +3525,30 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -3553,30 +3562,30 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>42</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -3591,24 +3600,24 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>24</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -3626,21 +3635,21 @@
         <v>48</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -3655,24 +3664,24 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -3690,21 +3699,21 @@
         <v>51</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -3722,15 +3731,15 @@
         <v>54</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -3745,18 +3754,18 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -3774,15 +3783,15 @@
         <v>64</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -3800,7 +3809,7 @@
         <v>65</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -3822,7 +3831,7 @@
         <v>66</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -3844,7 +3853,7 @@
         <v>67</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -3866,7 +3875,7 @@
         <v>68</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -3888,7 +3897,7 @@
         <v>69</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -3910,7 +3919,7 @@
         <v>70</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -3929,10 +3938,10 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="G26" s="4" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -3951,10 +3960,10 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="G27" s="4" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -3973,10 +3982,10 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="G28" s="4" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -3995,10 +4004,10 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="G29" s="4" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -4017,10 +4026,10 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="G30" s="4" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -4042,7 +4051,7 @@
         <v>71</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -4061,10 +4070,10 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -4083,10 +4092,10 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="G33" s="4" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -4105,10 +4114,10 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="G34" s="4" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -4130,7 +4139,7 @@
         <v>72</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -4149,10 +4158,10 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="G36" s="4" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -4171,10 +4180,10 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="G37" s="4" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -4193,10 +4202,10 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="G38" s="4" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -4215,10 +4224,10 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="G39" s="4" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -4237,10 +4246,10 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="G40" s="4" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -4259,10 +4268,10 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="G41" s="4" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -4281,10 +4290,10 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="G42" s="4" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -4303,10 +4312,10 @@
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="G43" s="4" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
@@ -4325,10 +4334,10 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="G44" s="4" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -4350,7 +4359,7 @@
         <v>73</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -4369,10 +4378,10 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="G46" s="4" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
@@ -4391,10 +4400,10 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="G47" s="4" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -4413,10 +4422,10 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="G48" s="4" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
@@ -4435,10 +4444,10 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="G49" s="4" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -4457,10 +4466,10 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="G50" s="4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
@@ -4479,10 +4488,10 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="G51" s="4" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
@@ -4504,7 +4513,7 @@
         <v>74</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
@@ -4523,10 +4532,10 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="G53" s="4" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
@@ -4545,10 +4554,10 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="G54" s="4" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
@@ -4567,10 +4576,10 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="G55" s="4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
@@ -4589,10 +4598,10 @@
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="G56" s="4" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
@@ -4611,10 +4620,10 @@
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="G57" s="4" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
@@ -4636,7 +4645,7 @@
         <v>75</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
@@ -4655,10 +4664,10 @@
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="G59" s="4" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
@@ -4677,10 +4686,10 @@
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="G60" s="4" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
@@ -4702,7 +4711,7 @@
         <v>76</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
@@ -4721,10 +4730,10 @@
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="G62" s="4" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
@@ -4743,10 +4752,10 @@
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="G63" s="4" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -4765,10 +4774,10 @@
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="G64" s="4" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
@@ -4787,10 +4796,10 @@
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
       <c r="G65" s="4" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
@@ -4809,10 +4818,10 @@
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
       <c r="G66" s="4" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
@@ -4834,7 +4843,7 @@
         <v>77</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
@@ -4896,17 +4905,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6" t="s">
@@ -4914,11 +4923,11 @@
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L1" s="6"/>
       <c r="M1" s="5" t="s">
@@ -4926,26 +4935,26 @@
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4956,37 +4965,37 @@
         <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="O2" s="4" t="n">
         <v>2016</v>
@@ -4996,55 +5005,55 @@
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="U2" s="4"/>
       <c r="V2" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="4" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
@@ -5052,40 +5061,40 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="4" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
@@ -5093,30 +5102,30 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="4" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
@@ -5130,36 +5139,36 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="4" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
@@ -5167,36 +5176,36 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="4" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
@@ -5205,24 +5214,24 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -5242,21 +5251,21 @@
         <v>38</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -5274,21 +5283,21 @@
         <v>39</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -5306,21 +5315,21 @@
         <v>40</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -5335,24 +5344,24 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -5370,21 +5379,21 @@
         <v>41</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>24</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -5402,21 +5411,21 @@
         <v>42</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -5431,24 +5440,24 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -5466,21 +5475,21 @@
         <v>45</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -5495,18 +5504,18 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -5521,18 +5530,18 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -5550,15 +5559,15 @@
         <v>47</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -5576,15 +5585,15 @@
         <v>48</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
@@ -5599,18 +5608,18 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="G21" s="4" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -5628,15 +5637,15 @@
         <v>49</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -5654,15 +5663,15 @@
         <v>50</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -5680,15 +5689,15 @@
         <v>51</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
@@ -5706,15 +5715,15 @@
         <v>52</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
@@ -5732,15 +5741,15 @@
         <v>53</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
@@ -5755,18 +5764,18 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="G27" s="4" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
@@ -5784,15 +5793,15 @@
         <v>54</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
@@ -5807,18 +5816,18 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="G29" s="4" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
@@ -5836,15 +5845,15 @@
         <v>55</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
@@ -5862,15 +5871,15 @@
         <v>56</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
@@ -5888,15 +5897,15 @@
         <v>57</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
@@ -5911,18 +5920,18 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="G33" s="4" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
@@ -5940,15 +5949,15 @@
         <v>58</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
@@ -5966,15 +5975,15 @@
         <v>59</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
@@ -5992,15 +6001,15 @@
         <v>60</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
@@ -6015,18 +6024,18 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="G37" s="4" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
@@ -6041,18 +6050,18 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="G38" s="4" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
@@ -6070,15 +6079,15 @@
         <v>61</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4" t="s">
-        <v>386</v>
+        <v>212</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
@@ -6096,7 +6105,7 @@
         <v>62</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -6118,7 +6127,7 @@
         <v>63</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -6137,10 +6146,10 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="G42" s="4" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -6162,7 +6171,7 @@
         <v>64</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
@@ -6184,7 +6193,7 @@
         <v>65</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -6206,7 +6215,7 @@
         <v>66</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -6228,7 +6237,7 @@
         <v>67</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
@@ -6250,7 +6259,7 @@
         <v>68</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -6272,7 +6281,7 @@
         <v>69</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
@@ -6294,7 +6303,7 @@
         <v>70</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -6313,10 +6322,10 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="G50" s="4" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
@@ -6335,10 +6344,10 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="G51" s="4" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
@@ -6357,10 +6366,10 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="G52" s="4" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
@@ -6379,10 +6388,10 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="G53" s="4" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
@@ -6401,10 +6410,10 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="G54" s="4" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
@@ -6426,7 +6435,7 @@
         <v>71</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
@@ -6445,10 +6454,10 @@
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="G56" s="4" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
@@ -6467,10 +6476,10 @@
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="G57" s="4" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
@@ -6489,10 +6498,10 @@
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="G58" s="4" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
@@ -6514,7 +6523,7 @@
         <v>72</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
@@ -6533,10 +6542,10 @@
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="G60" s="4" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
@@ -6555,10 +6564,10 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="G61" s="4" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
@@ -6577,10 +6586,10 @@
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="G62" s="4" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
@@ -6599,10 +6608,10 @@
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="G63" s="4" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -6621,10 +6630,10 @@
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="G64" s="4" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
@@ -6643,10 +6652,10 @@
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
       <c r="G65" s="4" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
@@ -6665,10 +6674,10 @@
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
       <c r="G66" s="4" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
@@ -6687,10 +6696,10 @@
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="G67" s="4" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
@@ -6709,10 +6718,10 @@
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="G68" s="4" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
@@ -6734,7 +6743,7 @@
         <v>73</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
@@ -6753,10 +6762,10 @@
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="G70" s="4" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
@@ -6775,10 +6784,10 @@
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
       <c r="G71" s="4" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
@@ -6797,10 +6806,10 @@
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
       <c r="G72" s="4" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
@@ -6819,10 +6828,10 @@
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
       <c r="G73" s="4" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
@@ -6841,10 +6850,10 @@
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
       <c r="G74" s="4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
@@ -6863,10 +6872,10 @@
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="G75" s="4" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
@@ -6888,7 +6897,7 @@
         <v>74</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
@@ -6907,10 +6916,10 @@
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
       <c r="G77" s="4" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
@@ -6929,10 +6938,10 @@
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
       <c r="G78" s="4" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
@@ -6951,10 +6960,10 @@
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
       <c r="G79" s="4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
@@ -6973,10 +6982,10 @@
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
       <c r="G80" s="4" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
@@ -6995,10 +7004,10 @@
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
       <c r="G81" s="4" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
@@ -7020,7 +7029,7 @@
         <v>75</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
@@ -7039,10 +7048,10 @@
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
       <c r="G83" s="4" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
@@ -7061,10 +7070,10 @@
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="G84" s="4" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
@@ -7086,7 +7095,7 @@
         <v>76</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I85" s="4"/>
       <c r="J85" s="4"/>
@@ -7105,10 +7114,10 @@
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
       <c r="G86" s="4" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
@@ -7127,10 +7136,10 @@
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
       <c r="G87" s="4" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
@@ -7149,10 +7158,10 @@
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
       <c r="G88" s="4" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
@@ -7171,10 +7180,10 @@
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
       <c r="G89" s="4" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="I89" s="4"/>
       <c r="J89" s="4"/>
@@ -7193,10 +7202,10 @@
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
       <c r="G90" s="4" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
@@ -7218,7 +7227,7 @@
         <v>77</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="I91" s="4"/>
       <c r="J91" s="4"/>

</xml_diff>

<commit_message>
[#50] working in Test [#82] pending to Test as output
[#50] Added MuSIASEM_EU_l_desc column (Visible in Test but not in Local)
[#82]  Matrix with interface flow information. Visible in test but can't see as output in Local NIS.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/08_caso_energia_eu_new_commands_CASE_SENSITIVE.xlsx
+++ b/backend_tests/z_input_files/v2/08_caso_energia_eu_new_commands_CASE_SENSITIVE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchies" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="392">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -67,48 +67,93 @@
     <t xml:space="preserve">AF</t>
   </si>
   <si>
+    <t xml:space="preserve">Agriculture/Forestry</t>
+  </si>
+  <si>
     <t xml:space="preserve">EM</t>
   </si>
   <si>
+    <t xml:space="preserve">Energy &amp; Mining</t>
+  </si>
+  <si>
     <t xml:space="preserve">FT</t>
   </si>
   <si>
+    <t xml:space="preserve">Food &amp; Tobacco</t>
+  </si>
+  <si>
     <t xml:space="preserve">TL</t>
   </si>
   <si>
+    <t xml:space="preserve">Textile &amp; Leather</t>
+  </si>
+  <si>
     <t xml:space="preserve">WWP</t>
   </si>
   <si>
+    <t xml:space="preserve">Wood &amp; Wood products</t>
+  </si>
+  <si>
     <t xml:space="preserve">PPP</t>
   </si>
   <si>
+    <t xml:space="preserve">Paper, Pulp &amp; Print</t>
+  </si>
+  <si>
     <t xml:space="preserve">CP</t>
   </si>
   <si>
+    <t xml:space="preserve">Chemical &amp; Petrochemical</t>
+  </si>
+  <si>
     <t xml:space="preserve">NS</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-specified (industry)</t>
+  </si>
+  <si>
     <t xml:space="preserve">NM</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-metallic Minerals</t>
+  </si>
+  <si>
     <t xml:space="preserve">BaM</t>
   </si>
   <si>
+    <t xml:space="preserve">Basic Metals</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ma</t>
   </si>
   <si>
+    <t xml:space="preserve">Machinery</t>
+  </si>
+  <si>
     <t xml:space="preserve">TE</t>
   </si>
   <si>
+    <t xml:space="preserve">Transport Equipment</t>
+  </si>
+  <si>
     <t xml:space="preserve">SGnT</t>
   </si>
   <si>
+    <t xml:space="preserve">Services (nT)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Co</t>
   </si>
   <si>
+    <t xml:space="preserve">Construction</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tr</t>
   </si>
   <si>
+    <t xml:space="preserve">Transport Services</t>
+  </si>
+  <si>
     <t xml:space="preserve">OriginDataset</t>
   </si>
   <si>
@@ -334,9 +379,6 @@
     <t xml:space="preserve">af</t>
   </si>
   <si>
-    <t xml:space="preserve">Agriculture/Forestry</t>
-  </si>
-  <si>
     <t xml:space="preserve">TIME_PERIOD</t>
   </si>
   <si>
@@ -373,9 +415,6 @@
     <t xml:space="preserve">Austria</t>
   </si>
   <si>
-    <t xml:space="preserve">Energy &amp; Mining</t>
-  </si>
-  <si>
     <t xml:space="preserve">FREQ</t>
   </si>
   <si>
@@ -403,9 +442,6 @@
     <t xml:space="preserve">Bosnia and Herzegovina</t>
   </si>
   <si>
-    <t xml:space="preserve">Food &amp; Tobacco</t>
-  </si>
-  <si>
     <t xml:space="preserve">UNIT</t>
   </si>
   <si>
@@ -433,9 +469,6 @@
     <t xml:space="preserve">Belgium</t>
   </si>
   <si>
-    <t xml:space="preserve">Textile &amp; Leather</t>
-  </si>
-  <si>
     <t xml:space="preserve">CLV_I10</t>
   </si>
   <si>
@@ -457,9 +490,6 @@
     <t xml:space="preserve">Bulgaria</t>
   </si>
   <si>
-    <t xml:space="preserve">Wood &amp; Wood products</t>
-  </si>
-  <si>
     <t xml:space="preserve">CLV_PCH_PRE</t>
   </si>
   <si>
@@ -484,9 +514,6 @@
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
-    <t xml:space="preserve">Paper, Pulp &amp; Print</t>
-  </si>
-  <si>
     <t xml:space="preserve">CP_MNAC</t>
   </si>
   <si>
@@ -508,9 +535,6 @@
     <t xml:space="preserve">Czech Republic</t>
   </si>
   <si>
-    <t xml:space="preserve">Chemical &amp; Petrochemical</t>
-  </si>
-  <si>
     <t xml:space="preserve">PD10_NAC</t>
   </si>
   <si>
@@ -526,9 +550,6 @@
     <t xml:space="preserve">Denmark</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-specified (industry)</t>
-  </si>
-  <si>
     <t xml:space="preserve">PD_PCH_PRE_EUR</t>
   </si>
   <si>
@@ -547,9 +568,6 @@
     <t xml:space="preserve">Euro area (EA11-2000, EA12-2006, EA13-2007, EA15-2008, EA16-2010, EA17-2013, EA18-2014, EA19)</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-metallic Minerals</t>
-  </si>
-  <si>
     <t xml:space="preserve">PD_PCH_PRE_NAC</t>
   </si>
   <si>
@@ -565,9 +583,6 @@
     <t xml:space="preserve">Euro area (12 countries)</t>
   </si>
   <si>
-    <t xml:space="preserve">Basic Metals</t>
-  </si>
-  <si>
     <t xml:space="preserve">PYP_MEUR</t>
   </si>
   <si>
@@ -583,9 +598,6 @@
     <t xml:space="preserve">Euro area (19 countries)</t>
   </si>
   <si>
-    <t xml:space="preserve">Machinery</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manufacture of rubber and plastic products</t>
   </si>
   <si>
@@ -595,9 +607,6 @@
     <t xml:space="preserve">European Union (15 countries)</t>
   </si>
   <si>
-    <t xml:space="preserve">Transport Equipment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manufacture of basic metals</t>
   </si>
   <si>
@@ -607,9 +616,6 @@
     <t xml:space="preserve">Finland</t>
   </si>
   <si>
-    <t xml:space="preserve">Services (nT)</t>
-  </si>
-  <si>
     <t xml:space="preserve">C24_C25</t>
   </si>
   <si>
@@ -622,9 +628,6 @@
     <t xml:space="preserve">France</t>
   </si>
   <si>
-    <t xml:space="preserve">Construction</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manufacture of electrical equipment</t>
   </si>
   <si>
@@ -632,9 +635,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ireland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport Services</t>
   </si>
   <si>
     <t xml:space="preserve">Manufacture of other transport equipment</t>
@@ -1349,7 +1349,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1415,13 +1415,25 @@
       <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,7 +1441,13 @@
         <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1437,7 +1455,13 @@
         <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,7 +1469,13 @@
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,7 +1483,13 @@
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1461,7 +1497,13 @@
         <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1469,7 +1511,13 @@
         <v>12</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,7 +1525,13 @@
         <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,7 +1539,13 @@
         <v>12</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,7 +1553,13 @@
         <v>12</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="K12" s="3"/>
     </row>
@@ -1502,7 +1568,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1512,7 +1584,13 @@
         <v>12</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1522,7 +1600,13 @@
         <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1532,7 +1616,13 @@
         <v>12</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1555,8 +1645,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1572,33 +1662,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>12</v>
@@ -1609,710 +1699,710 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>12</v>
@@ -2323,699 +2413,699 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="D71" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3059,8 +3149,8 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3068,15 +3158,18 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="13.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="13.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="23.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="75.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="3" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="55.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="47.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="20.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="3" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="3" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="16.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="3" width="25.28"/>
@@ -3086,29 +3179,29 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="L1" s="6"/>
       <c r="M1" s="5" t="s">
@@ -3116,67 +3209,67 @@
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="6" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="O2" s="4" t="n">
         <v>2016</v>
@@ -3186,55 +3279,55 @@
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="U2" s="4"/>
       <c r="V2" s="3" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="4" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
@@ -3242,40 +3335,40 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="4" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>126</v>
+        <v>18</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
@@ -3283,40 +3376,40 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="4" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
@@ -3324,40 +3417,40 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="4" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
@@ -3365,40 +3458,40 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="4" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>153</v>
+        <v>24</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
@@ -3408,34 +3501,34 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>161</v>
+        <v>26</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -3451,30 +3544,30 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>167</v>
+        <v>28</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -3488,30 +3581,30 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -3525,30 +3618,30 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -3562,30 +3655,30 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>186</v>
+        <v>34</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -3600,24 +3693,24 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>190</v>
+        <v>36</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -3632,24 +3725,24 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>194</v>
+        <v>38</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -3664,24 +3757,24 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>199</v>
+        <v>40</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -3696,24 +3789,24 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>203</v>
+        <v>42</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -3728,7 +3821,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>204</v>
@@ -3780,7 +3873,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>211</v>
@@ -3806,7 +3899,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="G20" s="4" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>214</v>
@@ -3828,7 +3921,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="G21" s="4" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>215</v>
@@ -3850,7 +3943,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>216</v>
@@ -3872,7 +3965,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>217</v>
@@ -3894,7 +3987,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="G24" s="4" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>218</v>
@@ -3916,7 +4009,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>219</v>
@@ -4048,7 +4141,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>230</v>
@@ -4136,7 +4229,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>237</v>
@@ -4356,7 +4449,7 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="G45" s="4" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>256</v>
@@ -4510,7 +4603,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="G52" s="4" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>269</v>
@@ -4642,7 +4735,7 @@
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="G58" s="4" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>280</v>
@@ -4708,7 +4801,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="G61" s="4" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>285</v>
@@ -4840,7 +4933,7 @@
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="G67" s="4" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="H67" s="4" t="s">
         <v>296</v>
@@ -4875,7 +4968,7 @@
   </sheetPr>
   <dimension ref="A1:V91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4905,29 +4998,29 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="L1" s="6"/>
       <c r="M1" s="5" t="s">
@@ -4935,37 +5028,37 @@
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="6" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>297</v>
@@ -4974,10 +5067,10 @@
         <v>298</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>299</v>
@@ -4986,16 +5079,16 @@
         <v>300</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="O2" s="4" t="n">
         <v>2016</v>
@@ -5005,13 +5098,13 @@
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="U2" s="4"/>
       <c r="V2" s="3" t="s">
@@ -5026,10 +5119,10 @@
         <v>303</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>304</v>
@@ -5038,22 +5131,22 @@
         <v>305</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
@@ -5067,10 +5160,10 @@
         <v>307</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>308</v>
@@ -5079,22 +5172,22 @@
         <v>309</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>126</v>
+        <v>18</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
@@ -5108,30 +5201,30 @@
         <v>311</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
@@ -5145,10 +5238,10 @@
         <v>313</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -5159,16 +5252,16 @@
         <v>315</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
@@ -5182,30 +5275,30 @@
         <v>317</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>153</v>
+        <v>24</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
@@ -5228,10 +5321,10 @@
         <v>321</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>161</v>
+        <v>26</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -5248,24 +5341,24 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>167</v>
+        <v>28</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -5280,7 +5373,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>322</v>
@@ -5288,16 +5381,16 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -5312,24 +5405,24 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -5344,24 +5437,24 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>186</v>
+        <v>34</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -5376,10 +5469,10 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -5390,10 +5483,10 @@
         <v>324</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>190</v>
+        <v>36</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -5408,10 +5501,10 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -5422,10 +5515,10 @@
         <v>326</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>194</v>
+        <v>38</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -5440,7 +5533,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>327</v>
@@ -5448,16 +5541,16 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>199</v>
+        <v>40</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -5472,7 +5565,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>328</v>
@@ -5486,10 +5579,10 @@
         <v>330</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>203</v>
+        <v>42</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -5504,10 +5597,10 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -5538,10 +5631,10 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -5556,7 +5649,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>335</v>
@@ -5564,10 +5657,10 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -5582,10 +5675,10 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="G20" s="4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -5608,10 +5701,10 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="G21" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -5634,7 +5727,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>340</v>
@@ -5642,10 +5735,10 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -5660,7 +5753,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>341</v>
@@ -5686,10 +5779,10 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="G24" s="4" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -5712,7 +5805,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>346</v>
@@ -5738,7 +5831,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="G26" s="4" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>349</v>
@@ -5790,7 +5883,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="G28" s="4" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>204</v>
@@ -5842,7 +5935,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="G30" s="4" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>360</v>
@@ -5868,7 +5961,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>363</v>
@@ -5894,7 +5987,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>366</v>
@@ -5946,7 +6039,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="G34" s="4" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>373</v>
@@ -5972,7 +6065,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>376</v>
@@ -5998,10 +6091,10 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="G36" s="4" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>199</v>
+        <v>40</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -6076,7 +6169,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="G39" s="4" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>389</v>
@@ -6102,7 +6195,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="G40" s="4" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>390</v>
@@ -6124,7 +6217,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="G41" s="4" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>391</v>
@@ -6168,7 +6261,7 @@
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="G43" s="4" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>211</v>
@@ -6190,7 +6283,7 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="G44" s="4" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>214</v>
@@ -6212,7 +6305,7 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="G45" s="4" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>215</v>
@@ -6234,7 +6327,7 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="G46" s="4" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>216</v>
@@ -6256,7 +6349,7 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="G47" s="4" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>217</v>
@@ -6278,7 +6371,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="G48" s="4" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>218</v>
@@ -6300,7 +6393,7 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="G49" s="4" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>219</v>
@@ -6432,7 +6525,7 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="G55" s="4" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>230</v>
@@ -6520,7 +6613,7 @@
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="G59" s="4" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>237</v>
@@ -6740,7 +6833,7 @@
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="G69" s="4" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>256</v>
@@ -6894,7 +6987,7 @@
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="G76" s="4" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>269</v>
@@ -7026,7 +7119,7 @@
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
       <c r="G82" s="4" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>280</v>
@@ -7092,7 +7185,7 @@
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
       <c r="G85" s="4" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H85" s="4" t="s">
         <v>285</v>
@@ -7224,7 +7317,7 @@
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
       <c r="G91" s="4" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="H91" s="4" t="s">
         <v>296</v>

</xml_diff>

<commit_message>
label in DatasetQry result
Added Hierarchy label in the DatasetQry output
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/08_caso_energia_eu_new_commands_CASE_SENSITIVE.xlsx
+++ b/backend_tests/z_input_files/v2/08_caso_energia_eu_new_commands_CASE_SENSITIVE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchies" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="392">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -1348,8 +1348,8 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1361,7 +1361,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.43"/>
@@ -1418,9 +1418,7 @@
       <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="3" t="s">
@@ -1432,9 +1430,7 @@
       <c r="H3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="3" t="s">
@@ -1446,9 +1442,7 @@
       <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="3" t="s">
@@ -1460,9 +1454,7 @@
       <c r="H5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="3" t="s">
@@ -1474,9 +1466,7 @@
       <c r="H6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="3" t="s">
@@ -1488,9 +1478,7 @@
       <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="3" t="s">
@@ -1502,9 +1490,7 @@
       <c r="H8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="3" t="s">
@@ -1516,9 +1502,7 @@
       <c r="H9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="3" t="s">
@@ -1530,9 +1514,7 @@
       <c r="H10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="3" t="s">
@@ -1544,9 +1526,7 @@
       <c r="H11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="3" t="s">
@@ -1558,9 +1538,7 @@
       <c r="H12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="I12" s="3"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,9 +1551,7 @@
       <c r="H13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
@@ -1589,9 +1565,7 @@
       <c r="H14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
@@ -1605,9 +1579,7 @@
       <c r="H15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
@@ -1621,9 +1593,7 @@
       <c r="H16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
@@ -3149,7 +3119,7 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>

</xml_diff>